<commit_message>
Continuous development on the analysis Continuous development on the analysis  and added some charts
</commit_message>
<xml_diff>
--- a/misc/charts.xlsx
+++ b/misc/charts.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edrick\PycharmProjects\pythonProject\twse_sq_scraper\misc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dickl\VSCode_Project\TWSE_ShortQuotaScrape\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E80D980C-0261-434B-9E88-350BF3334F06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F23AC51E-DB1D-49F9-B241-E088613255D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11184" yWindow="4788" windowWidth="19440" windowHeight="11412" activeTab="1" xr2:uid="{ECAD5CE7-5018-4594-B03C-C58688BCC4BE}"/>
+    <workbookView xWindow="-100" yWindow="-100" windowWidth="21467" windowHeight="11443" activeTab="3" xr2:uid="{ECAD5CE7-5018-4594-B03C-C58688BCC4BE}"/>
   </bookViews>
   <sheets>
     <sheet name="daily_used_sq" sheetId="1" r:id="rId1"/>
     <sheet name="stk_avg_quota_used" sheetId="2" r:id="rId2"/>
     <sheet name="stk_avg_transaction" sheetId="3" r:id="rId3"/>
+    <sheet name="stk_avg_turnover" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">stk_avg_quota_used!$A$2:$B$2</definedName>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="101">
   <si>
     <t>dates</t>
   </si>
@@ -339,11 +340,20 @@
   <si>
     <t>3049</t>
   </si>
+  <si>
+    <t>Shares turnover</t>
+  </si>
+  <si>
+    <t>Note: Before market close there will be abnormal move in individual stocks, but overall the effect is muted</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -538,7 +548,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -576,6 +586,12 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -594,12 +610,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -874,7 +885,7 @@
             </c:layout>
             <c:tx>
               <c:rich>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
@@ -902,7 +913,7 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -979,6 +990,344 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.5892746934169539E-2"/>
+          <c:y val="0.16245370370370371"/>
+          <c:w val="0.79883077958643667"/>
+          <c:h val="0.73477653834937295"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="002060"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>stk_avg_turnover!$B$3:$B$10</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>8-9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9-10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10-11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11-12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12-13</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13-14</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14-15</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15-16</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>stk_avg_turnover!$C$3:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>340223141.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6639275502.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4679403378</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4142568385.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3019092058</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2184713577</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1323342.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>485520</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C145-42CA-B82A-CC4082781F2B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="76"/>
+        <c:overlap val="54"/>
+        <c:axId val="595658248"/>
+        <c:axId val="449979896"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="595658248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="449979896"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="449979896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="98000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="595658248"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:dispUnits>
+          <c:builtInUnit val="millions"/>
+          <c:dispUnitsLbl>
+            <c:layout>
+              <c:manualLayout>
+                <c:xMode val="edge"/>
+                <c:yMode val="edge"/>
+                <c:x val="1.714192382744412E-2"/>
+                <c:y val="3.2824074074074075E-2"/>
+              </c:manualLayout>
+            </c:layout>
+            <c:tx>
+              <c:rich>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:sysClr val="windowText" lastClr="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:r>
+                    <a:rPr lang="en-US"/>
+                    <a:t>Mil</a:t>
+                  </a:r>
+                </a:p>
+              </c:rich>
+            </c:tx>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+          </c:dispUnitsLbl>
+        </c:dispUnits>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId3"/>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1019,7 +1368,550 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1563,6 +2455,161 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>21102</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>182878</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>335281</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>182878</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A97FA682-D1E4-419A-B316-ACDC696D2C83}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.0893</cdr:x>
+      <cdr:y>7.29076E-7</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.9672</cdr:x>
+      <cdr:y>0.11282</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4EC1E946-AF3E-2E44-31CD-E8984FC959B2}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="414997" y="2"/>
+          <a:ext cx="4079631" cy="309489"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="1" i="0" u="sng" baseline="0">
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Total number of shares traded in each hour</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-HK" sz="1600">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.86428</cdr:x>
+      <cdr:y>0.89744</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>1</cdr:x>
+      <cdr:y>0.98205</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C9EC3EA-272A-4370-0FCE-923BCEDCC2B4}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="4016326" y="2461847"/>
+          <a:ext cx="630702" cy="232116"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-HK" sz="1050"/>
+            <a:t>AM/PM</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1868,7 +2915,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="2:3" x14ac:dyDescent="0.3">
@@ -1919,35 +2966,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B804F25-E67C-4FBB-8032-AA2B519A402F}">
   <dimension ref="A1:H1640"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.3984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" customWidth="1"/>
-    <col min="6" max="6" width="14.5546875" customWidth="1"/>
+    <col min="6" max="6" width="14.59765625" customWidth="1"/>
     <col min="7" max="7" width="8" customWidth="1"/>
-    <col min="8" max="8" width="14.5546875" customWidth="1"/>
+    <col min="8" max="8" width="14.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="14.95" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:8" ht="14.95" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="17"/>
-    </row>
-    <row r="3" spans="1:8" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="19"/>
+    </row>
+    <row r="3" spans="1:8" ht="3.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1983,19 +3030,19 @@
         <v>-0.99896466815802198</v>
       </c>
       <c r="E5" s="4" t="str">
-        <f>A4</f>
+        <f t="shared" ref="E5:E14" si="0">A4</f>
         <v>0056</v>
       </c>
       <c r="F5" s="5">
-        <f>-B4</f>
+        <f t="shared" ref="F5:F14" si="1">-B4</f>
         <v>0.99991535888373995</v>
       </c>
       <c r="G5" s="6" t="str">
-        <f>A14</f>
+        <f t="shared" ref="G5:G14" si="2">A14</f>
         <v>2609</v>
       </c>
       <c r="H5" s="7">
-        <f>-B14</f>
+        <f t="shared" ref="H5:H14" si="3">-B14</f>
         <v>0.99163993047155197</v>
       </c>
     </row>
@@ -2007,19 +3054,19 @@
         <v>-0.99799916382195297</v>
       </c>
       <c r="E6" s="4" t="str">
-        <f>A5</f>
+        <f t="shared" si="0"/>
         <v>2486</v>
       </c>
       <c r="F6" s="5">
-        <f>-B5</f>
+        <f t="shared" si="1"/>
         <v>0.99896466815802198</v>
       </c>
       <c r="G6" s="6" t="str">
-        <f>A15</f>
+        <f t="shared" si="2"/>
         <v>2006</v>
       </c>
       <c r="H6" s="7">
-        <f>-B15</f>
+        <f t="shared" si="3"/>
         <v>0.98778935628972697</v>
       </c>
     </row>
@@ -2031,19 +3078,19 @@
         <v>-0.997992003904561</v>
       </c>
       <c r="E7" s="4" t="str">
-        <f>A6</f>
+        <f t="shared" si="0"/>
         <v>3034</v>
       </c>
       <c r="F7" s="5">
-        <f>-B6</f>
+        <f t="shared" si="1"/>
         <v>0.99799916382195297</v>
       </c>
       <c r="G7" s="6" t="str">
-        <f>A16</f>
+        <f t="shared" si="2"/>
         <v>3036</v>
       </c>
       <c r="H7" s="7">
-        <f>-B16</f>
+        <f t="shared" si="3"/>
         <v>0.98737600384424196</v>
       </c>
     </row>
@@ -2055,19 +3102,19 @@
         <v>-0.99679892344770904</v>
       </c>
       <c r="E8" s="4" t="str">
-        <f>A7</f>
+        <f t="shared" si="0"/>
         <v>2441</v>
       </c>
       <c r="F8" s="5">
-        <f>-B7</f>
+        <f t="shared" si="1"/>
         <v>0.997992003904561</v>
       </c>
       <c r="G8" s="6" t="str">
-        <f>A17</f>
+        <f t="shared" si="2"/>
         <v>00900</v>
       </c>
       <c r="H8" s="7">
-        <f>-B17</f>
+        <f t="shared" si="3"/>
         <v>0.98709891722082799</v>
       </c>
     </row>
@@ -2079,19 +3126,19 @@
         <v>-0.99532557737430505</v>
       </c>
       <c r="E9" s="4" t="str">
-        <f>A8</f>
+        <f t="shared" si="0"/>
         <v>6505</v>
       </c>
       <c r="F9" s="5">
-        <f>-B8</f>
+        <f t="shared" si="1"/>
         <v>0.99679892344770904</v>
       </c>
       <c r="G9" s="6" t="str">
-        <f>A18</f>
+        <f t="shared" si="2"/>
         <v>1303</v>
       </c>
       <c r="H9" s="7">
-        <f>-B18</f>
+        <f t="shared" si="3"/>
         <v>0.984045787150021</v>
       </c>
     </row>
@@ -2103,19 +3150,19 @@
         <v>-0.99403112049493103</v>
       </c>
       <c r="E10" s="4" t="str">
-        <f>A9</f>
+        <f t="shared" si="0"/>
         <v>3576</v>
       </c>
       <c r="F10" s="5">
-        <f>-B9</f>
+        <f t="shared" si="1"/>
         <v>0.99532557737430505</v>
       </c>
       <c r="G10" s="6" t="str">
-        <f>A19</f>
+        <f t="shared" si="2"/>
         <v>2539</v>
       </c>
       <c r="H10" s="7">
-        <f>-B19</f>
+        <f t="shared" si="3"/>
         <v>0.98396963811670901</v>
       </c>
     </row>
@@ -2127,19 +3174,19 @@
         <v>-0.99383420633810904</v>
       </c>
       <c r="E11" s="4" t="str">
-        <f>A10</f>
+        <f t="shared" si="0"/>
         <v>2356</v>
       </c>
       <c r="F11" s="5">
-        <f>-B10</f>
+        <f t="shared" si="1"/>
         <v>0.99403112049493103</v>
       </c>
       <c r="G11" s="6" t="str">
-        <f>A20</f>
+        <f t="shared" si="2"/>
         <v>2881</v>
       </c>
       <c r="H11" s="7">
-        <f>-B20</f>
+        <f t="shared" si="3"/>
         <v>0.98377130059621698</v>
       </c>
     </row>
@@ -2151,19 +3198,19 @@
         <v>-0.99308746725049102</v>
       </c>
       <c r="E12" s="4" t="str">
-        <f>A11</f>
+        <f t="shared" si="0"/>
         <v>1455</v>
       </c>
       <c r="F12" s="5">
-        <f>-B11</f>
+        <f t="shared" si="1"/>
         <v>0.99383420633810904</v>
       </c>
       <c r="G12" s="6" t="str">
-        <f>A21</f>
+        <f t="shared" si="2"/>
         <v>1304</v>
       </c>
       <c r="H12" s="7">
-        <f>-B21</f>
+        <f t="shared" si="3"/>
         <v>0.98207194437435796</v>
       </c>
     </row>
@@ -2175,23 +3222,23 @@
         <v>-0.99179535331397195</v>
       </c>
       <c r="E13" s="4" t="str">
-        <f>A12</f>
+        <f t="shared" si="0"/>
         <v>8926</v>
       </c>
       <c r="F13" s="5">
-        <f>-B12</f>
+        <f t="shared" si="1"/>
         <v>0.99308746725049102</v>
       </c>
       <c r="G13" s="6" t="str">
-        <f>A22</f>
+        <f t="shared" si="2"/>
         <v>1718</v>
       </c>
       <c r="H13" s="7">
-        <f>-B22</f>
+        <f t="shared" si="3"/>
         <v>0.97905310189579597</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="14.95" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>35</v>
       </c>
@@ -2199,35 +3246,35 @@
         <v>-0.99163993047155197</v>
       </c>
       <c r="E14" s="8" t="str">
-        <f>A13</f>
+        <f t="shared" si="0"/>
         <v>1314</v>
       </c>
       <c r="F14" s="9">
-        <f>-B13</f>
+        <f t="shared" si="1"/>
         <v>0.99179535331397195</v>
       </c>
       <c r="G14" s="10" t="str">
-        <f>A23</f>
+        <f t="shared" si="2"/>
         <v>2412</v>
       </c>
       <c r="H14" s="11">
-        <f>-B23</f>
+        <f t="shared" si="3"/>
         <v>0.97626400178408801</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="28.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>74</v>
       </c>
       <c r="B15" s="2">
         <v>-0.98778935628972697</v>
       </c>
-      <c r="E15" s="18" t="s">
+      <c r="E15" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
@@ -8900,29 +9947,29 @@
   <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="20.33203125" customWidth="1"/>
+    <col min="6" max="6" width="20.296875" customWidth="1"/>
     <col min="7" max="7" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="14.95" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:7" ht="14.95" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="20"/>
-    </row>
-    <row r="3" spans="1:7" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+      <c r="G2" s="22"/>
+    </row>
+    <row r="3" spans="1:7" ht="3.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>35</v>
@@ -8945,11 +9992,11 @@
         <v>199.25</v>
       </c>
       <c r="F5" s="4" t="str">
-        <f>A4</f>
+        <f t="shared" ref="F5:F14" si="0">A4</f>
         <v>2609</v>
       </c>
-      <c r="G5" s="21">
-        <f>B4</f>
+      <c r="G5" s="15">
+        <f t="shared" ref="G5:G14" si="1">B4</f>
         <v>222.25</v>
       </c>
     </row>
@@ -8961,11 +10008,11 @@
         <v>195.5</v>
       </c>
       <c r="F6" s="4" t="str">
-        <f>A5</f>
+        <f t="shared" si="0"/>
         <v>00878</v>
       </c>
-      <c r="G6" s="21">
-        <f>B5</f>
+      <c r="G6" s="15">
+        <f t="shared" si="1"/>
         <v>199.25</v>
       </c>
     </row>
@@ -8977,11 +10024,11 @@
         <v>190.25</v>
       </c>
       <c r="F7" s="4" t="str">
-        <f>A6</f>
+        <f t="shared" si="0"/>
         <v>006208</v>
       </c>
-      <c r="G7" s="21">
-        <f>B6</f>
+      <c r="G7" s="15">
+        <f t="shared" si="1"/>
         <v>195.5</v>
       </c>
     </row>
@@ -8993,11 +10040,11 @@
         <v>186.5</v>
       </c>
       <c r="F8" s="4" t="str">
-        <f>A7</f>
+        <f t="shared" si="0"/>
         <v>00636</v>
       </c>
-      <c r="G8" s="21">
-        <f>B7</f>
+      <c r="G8" s="15">
+        <f t="shared" si="1"/>
         <v>190.25</v>
       </c>
     </row>
@@ -9009,11 +10056,11 @@
         <v>182.25</v>
       </c>
       <c r="F9" s="4" t="str">
-        <f>A8</f>
+        <f t="shared" si="0"/>
         <v>4123</v>
       </c>
-      <c r="G9" s="21">
-        <f>B8</f>
+      <c r="G9" s="15">
+        <f t="shared" si="1"/>
         <v>186.5</v>
       </c>
     </row>
@@ -9025,11 +10072,11 @@
         <v>179.25</v>
       </c>
       <c r="F10" s="4" t="str">
-        <f>A9</f>
+        <f t="shared" si="0"/>
         <v>00655L</v>
       </c>
-      <c r="G10" s="21">
-        <f>B9</f>
+      <c r="G10" s="15">
+        <f t="shared" si="1"/>
         <v>182.25</v>
       </c>
     </row>
@@ -9041,11 +10088,11 @@
         <v>176.25</v>
       </c>
       <c r="F11" s="4" t="str">
-        <f>A10</f>
+        <f t="shared" si="0"/>
         <v>2303</v>
       </c>
-      <c r="G11" s="21">
-        <f>B10</f>
+      <c r="G11" s="15">
+        <f t="shared" si="1"/>
         <v>179.25</v>
       </c>
     </row>
@@ -9057,11 +10104,11 @@
         <v>167.75</v>
       </c>
       <c r="F12" s="4" t="str">
-        <f>A11</f>
+        <f t="shared" si="0"/>
         <v>2317</v>
       </c>
-      <c r="G12" s="21">
-        <f>B11</f>
+      <c r="G12" s="15">
+        <f t="shared" si="1"/>
         <v>176.25</v>
       </c>
     </row>
@@ -9073,15 +10120,15 @@
         <v>162</v>
       </c>
       <c r="F13" s="4" t="str">
-        <f>A12</f>
+        <f t="shared" si="0"/>
         <v>2610</v>
       </c>
-      <c r="G13" s="21">
-        <f>B12</f>
+      <c r="G13" s="15">
+        <f t="shared" si="1"/>
         <v>167.75</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" ht="14.95" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>41</v>
       </c>
@@ -9089,11 +10136,11 @@
         <v>161.5</v>
       </c>
       <c r="F14" s="8" t="str">
-        <f>A13</f>
+        <f t="shared" si="0"/>
         <v>6180</v>
       </c>
-      <c r="G14" s="22">
-        <f>B13</f>
+      <c r="G14" s="16">
+        <f t="shared" si="1"/>
         <v>162</v>
       </c>
     </row>
@@ -9104,8 +10151,8 @@
       <c r="B15">
         <v>159.75</v>
       </c>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
@@ -9418,4 +10465,132 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4441B833-2C01-4754-85AE-9EFE5DC7796E}">
+  <dimension ref="A2:E20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="11.296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="23">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="23">
+        <v>0.375</v>
+      </c>
+      <c r="B3" s="23" t="str">
+        <f>TEXT(A2,"h")&amp;"-"&amp;TEXT(A3,"h")</f>
+        <v>8-9</v>
+      </c>
+      <c r="C3">
+        <v>340223141.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="23">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="B4" s="23" t="str">
+        <f t="shared" ref="B4:B10" si="0">TEXT(A3,"h")&amp;"-"&amp;TEXT(A4,"h")</f>
+        <v>9-10</v>
+      </c>
+      <c r="C4">
+        <v>6639275502.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="23">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="B5" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>10-11</v>
+      </c>
+      <c r="C5">
+        <v>4679403378</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="B6" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>11-12</v>
+      </c>
+      <c r="C6">
+        <v>4142568385.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="23">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="B7" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>12-13</v>
+      </c>
+      <c r="C7">
+        <v>3019092058</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="23">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="B8" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>13-14</v>
+      </c>
+      <c r="C8">
+        <v>2184713577</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="23">
+        <v>0.625</v>
+      </c>
+      <c r="B9" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>14-15</v>
+      </c>
+      <c r="C9">
+        <v>1323342.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="23">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="B10" s="23" t="str">
+        <f t="shared" si="0"/>
+        <v>15-16</v>
+      </c>
+      <c r="C10">
+        <v>485520</v>
+      </c>
+    </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added comments on UTC time consideration
</commit_message>
<xml_diff>
--- a/misc/charts.xlsx
+++ b/misc/charts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edrick\PycharmProjects\pythonProject\twse_sq_scraper\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9C3A245-3165-497B-B4D6-FF482A215515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68128C8C-3F84-4694-9295-828270DD8507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14712" yWindow="2340" windowWidth="14388" windowHeight="13404" xr2:uid="{ECAD5CE7-5018-4594-B03C-C58688BCC4BE}"/>
+    <workbookView xWindow="14712" yWindow="2340" windowWidth="14388" windowHeight="13404" firstSheet="1" activeTab="3" xr2:uid="{ECAD5CE7-5018-4594-B03C-C58688BCC4BE}"/>
   </bookViews>
   <sheets>
     <sheet name="daily_used_sq" sheetId="1" r:id="rId1"/>
@@ -624,20 +624,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -661,13 +649,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -676,7 +658,25 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4626,7 +4626,7 @@
               <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>tocks with transaction before 8:55am on are removed </a:t>
+            <a:t>tocks with transaction before 8:55am are removed </a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -4798,7 +4798,7 @@
               <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>tocks with transaction before 8:55am on are removed </a:t>
+            <a:t>tocks with transaction before 8:55am are removed </a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -40487,8 +40487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF7EF5E0-FE04-458C-ADB6-192872593107}">
   <dimension ref="B6:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -40569,12 +40569,12 @@
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="18"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="30"/>
     </row>
     <row r="3" spans="1:8" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -40851,12 +40851,12 @@
       <c r="B15" s="2">
         <v>-0.98778935628972697</v>
       </c>
-      <c r="E15" s="19" t="s">
+      <c r="E15" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="31"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
@@ -47546,27 +47546,27 @@
       <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="29" t="s">
+      <c r="F2" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
     </row>
     <row r="3" spans="1:8" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:8" s="23" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="22" t="s">
+    <row r="4" spans="1:8" s="19" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="23">
+      <c r="B4" s="19">
         <v>222.25</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="25" t="s">
+      <c r="G4" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="25" t="s">
+      <c r="H4" s="21" t="s">
         <v>103</v>
       </c>
     </row>
@@ -47581,11 +47581,11 @@
         <f t="shared" ref="F5:F14" si="0">A4</f>
         <v>2609</v>
       </c>
-      <c r="G5" s="21">
+      <c r="G5" s="17">
         <f t="shared" ref="G5:G14" si="1">B4</f>
         <v>222.25</v>
       </c>
-      <c r="H5" s="26">
+      <c r="H5" s="22">
         <f>VLOOKUP($F5,[1]stk_short_int_ratio!$A$1:$F$1797,2,0)</f>
         <v>4.7757893808431824E-2</v>
       </c>
@@ -47601,11 +47601,11 @@
         <f t="shared" si="0"/>
         <v>00878</v>
       </c>
-      <c r="G6" s="21">
+      <c r="G6" s="17">
         <f t="shared" si="1"/>
         <v>199.25</v>
       </c>
-      <c r="H6" s="26">
+      <c r="H6" s="22">
         <f>VLOOKUP($F6,[1]stk_short_int_ratio!$A$1:$F$1797,2,0)</f>
         <v>1.2956322579265708E-2</v>
       </c>
@@ -47621,11 +47621,11 @@
         <f t="shared" si="0"/>
         <v>006208</v>
       </c>
-      <c r="G7" s="21">
+      <c r="G7" s="17">
         <f t="shared" si="1"/>
         <v>195.5</v>
       </c>
-      <c r="H7" s="26">
+      <c r="H7" s="22">
         <f>VLOOKUP($F7,[1]stk_short_int_ratio!$A$1:$F$1797,2,0)</f>
         <v>8.0444623589234782E-3</v>
       </c>
@@ -47641,11 +47641,11 @@
         <f t="shared" si="0"/>
         <v>00636</v>
       </c>
-      <c r="G8" s="21">
+      <c r="G8" s="17">
         <f t="shared" si="1"/>
         <v>190.25</v>
       </c>
-      <c r="H8" s="26">
+      <c r="H8" s="22">
         <f>VLOOKUP($F8,[1]stk_short_int_ratio!$A$1:$F$1797,2,0)</f>
         <v>1.1724968805128867E-2</v>
       </c>
@@ -47661,11 +47661,11 @@
         <f t="shared" si="0"/>
         <v>4123</v>
       </c>
-      <c r="G9" s="21">
+      <c r="G9" s="17">
         <f t="shared" si="1"/>
         <v>186.5</v>
       </c>
-      <c r="H9" s="26">
+      <c r="H9" s="22">
         <f>VLOOKUP($F9,[1]stk_short_int_ratio!$A$1:$F$1797,2,0)</f>
         <v>5.5484938361277569E-5</v>
       </c>
@@ -47681,11 +47681,11 @@
         <f t="shared" si="0"/>
         <v>00655L</v>
       </c>
-      <c r="G10" s="21">
+      <c r="G10" s="17">
         <f t="shared" si="1"/>
         <v>182.25</v>
       </c>
-      <c r="H10" s="26">
+      <c r="H10" s="22">
         <f>VLOOKUP($F10,[1]stk_short_int_ratio!$A$1:$F$1797,2,0)</f>
         <v>1.7964323542762992E-2</v>
       </c>
@@ -47701,11 +47701,11 @@
         <f t="shared" si="0"/>
         <v>2303</v>
       </c>
-      <c r="G11" s="21">
+      <c r="G11" s="17">
         <f t="shared" si="1"/>
         <v>179.25</v>
       </c>
-      <c r="H11" s="26">
+      <c r="H11" s="22">
         <f>VLOOKUP($F11,[1]stk_short_int_ratio!$A$1:$F$1797,2,0)</f>
         <v>5.3876990776088825E-2</v>
       </c>
@@ -47721,11 +47721,11 @@
         <f t="shared" si="0"/>
         <v>2317</v>
       </c>
-      <c r="G12" s="21">
+      <c r="G12" s="17">
         <f t="shared" si="1"/>
         <v>176.25</v>
       </c>
-      <c r="H12" s="26">
+      <c r="H12" s="22">
         <f>VLOOKUP($F12,[1]stk_short_int_ratio!$A$1:$F$1797,2,0)</f>
         <v>3.0414782813808564E-3</v>
       </c>
@@ -47741,11 +47741,11 @@
         <f t="shared" si="0"/>
         <v>2610</v>
       </c>
-      <c r="G13" s="21">
+      <c r="G13" s="17">
         <f t="shared" si="1"/>
         <v>167.75</v>
       </c>
-      <c r="H13" s="26">
+      <c r="H13" s="22">
         <f>VLOOKUP($F13,[1]stk_short_int_ratio!$A$1:$F$1797,2,0)</f>
         <v>5.4543939116031059E-2</v>
       </c>
@@ -47761,11 +47761,11 @@
         <f t="shared" si="0"/>
         <v>6180</v>
       </c>
-      <c r="G14" s="27">
+      <c r="G14" s="23">
         <f t="shared" si="1"/>
         <v>162</v>
       </c>
-      <c r="H14" s="28">
+      <c r="H14" s="24">
         <f>VLOOKUP($F14,[1]stk_short_int_ratio!$A$1:$F$1797,2,0)</f>
         <v>4.5015886619227137E-4</v>
       </c>
@@ -47777,13 +47777,13 @@
       <c r="B15">
         <v>159.75</v>
       </c>
-      <c r="F15" s="33" t="s">
+      <c r="F15" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="G15" s="31" t="s">
+      <c r="G15" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="H15" s="32">
+      <c r="H15" s="26">
         <f>[1]stk_short_int_ratio!$B$1</f>
         <v>8.6099189377924473E-3</v>
       </c>
@@ -48111,8 +48111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4441B833-2C01-4754-85AE-9EFE5DC7796E}">
   <dimension ref="A2:G50"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -48254,7 +48254,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="20">
+      <c r="A29" s="16">
         <v>0.375</v>
       </c>
       <c r="B29">
@@ -48279,7 +48279,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="20">
+      <c r="A30" s="16">
         <v>0.41666666666666669</v>
       </c>
       <c r="B30">
@@ -48304,7 +48304,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="20">
+      <c r="A31" s="16">
         <v>0.45833333333333331</v>
       </c>
       <c r="B31">
@@ -48329,7 +48329,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="20">
+      <c r="A32" s="16">
         <v>0.5</v>
       </c>
       <c r="B32">
@@ -48354,7 +48354,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="20">
+      <c r="A33" s="16">
         <v>0.54166666666666663</v>
       </c>
       <c r="B33">
@@ -48379,7 +48379,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="20">
+      <c r="A34" s="16">
         <v>0.58333333333333337</v>
       </c>
       <c r="B34">
@@ -48404,7 +48404,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="20">
+      <c r="A35" s="16">
         <v>0.625</v>
       </c>
       <c r="B35">
@@ -48429,7 +48429,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="20">
+      <c r="A36" s="16">
         <v>0.66666666666666663</v>
       </c>
       <c r="B36">
@@ -48473,7 +48473,7 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="20">
+      <c r="A43" s="16">
         <v>0.375</v>
       </c>
       <c r="B43">
@@ -48498,7 +48498,7 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="20">
+      <c r="A44" s="16">
         <v>0.41666666666666669</v>
       </c>
       <c r="B44">
@@ -48523,7 +48523,7 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="20">
+      <c r="A45" s="16">
         <v>0.45833333333333331</v>
       </c>
       <c r="B45">
@@ -48548,7 +48548,7 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="20">
+      <c r="A46" s="16">
         <v>0.5</v>
       </c>
       <c r="B46">
@@ -48573,7 +48573,7 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="20">
+      <c r="A47" s="16">
         <v>0.54166666666666663</v>
       </c>
       <c r="B47">
@@ -48598,7 +48598,7 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="20">
+      <c r="A48" s="16">
         <v>0.58333333333333337</v>
       </c>
       <c r="B48">
@@ -48623,7 +48623,7 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="20">
+      <c r="A49" s="16">
         <v>0.625</v>
       </c>
       <c r="B49">
@@ -48648,7 +48648,7 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="20">
+      <c r="A50" s="16">
         <v>0.66666666666666663</v>
       </c>
       <c r="B50">

</xml_diff>